<commit_message>
fix : comments and xml documentation
</commit_message>
<xml_diff>
--- a/instances/UNCHECKED instance + resultat MIP/Synthese.xlsx
+++ b/instances/UNCHECKED instance + resultat MIP/Synthese.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benhi\source\repos\BiLevel_Scheduling_Industry_4.0\instances\UNCHECKED instance + resultat MIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6019C784-A80F-4167-A346-DBD53B0A91C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E7B3174E-097B-442E-B67C-695A83B1DEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resultSPT_VL_LATE2EARLY_Synth" sheetId="9" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="resultLPT_DUMB_Synth" sheetId="2" r:id="rId8"/>
     <sheet name="resultMIP_Synth" sheetId="11" r:id="rId9"/>
     <sheet name="DUMB" sheetId="1" r:id="rId10"/>
-    <sheet name="LATE2EARLY" sheetId="10" r:id="rId11"/>
+    <sheet name="InstanceDifficiles" sheetId="12" r:id="rId11"/>
+    <sheet name="LATE2EARLY" sheetId="10" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="DonnéesExternes_1" localSheetId="7" hidden="1">'resultLPT_DUMB_Synth'!$A$1:$K$19</definedName>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="177" uniqueCount="21">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="245" uniqueCount="27">
   <si>
     <t>N</t>
   </si>
@@ -156,6 +157,24 @@
   <si>
     <t>#OPT/MIP (%)</t>
   </si>
+  <si>
+    <t>N:15 n:7 m:4 #inst:375</t>
+  </si>
+  <si>
+    <t>N:20 n:10 m:4 #inst:375</t>
+  </si>
+  <si>
+    <t>N:30 n:15 m:4 #inst:375</t>
+  </si>
+  <si>
+    <t>N:30 n:7 m:4 #inst:375</t>
+  </si>
+  <si>
+    <t>NomHeuristique</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
@@ -198,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <start/>
       <end/>
@@ -401,11 +420,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -422,6 +456,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,19 +472,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1830,8 +1866,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H32" zoomScale="71" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView topLeftCell="A28" zoomScale="71" workbookViewId="0">
+      <selection activeCell="A53" activeCellId="7" sqref="A34:XFD34 A37:XFD37 A40:XFD40 A41:XFD41 A60:XFD60 A59:XFD59 A56:XFD56 A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2112,36 +2148,36 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="16" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="16" t="s">
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="16" t="s">
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="25" t="s">
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
@@ -2192,16 +2228,16 @@
       <c r="Q24" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R24" s="19" t="s">
+      <c r="R24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="S24" s="19" t="s">
+      <c r="S24" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="T24" s="19" t="s">
+      <c r="T24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="U24" s="20" t="s">
+      <c r="U24" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2258,16 +2294,16 @@
       <c r="Q25" s="12">
         <v>0.04</v>
       </c>
-      <c r="R25" s="21">
+      <c r="R25" s="18">
         <v>125</v>
       </c>
-      <c r="S25" s="21">
+      <c r="S25" s="18">
         <v>7.4087700000000005</v>
       </c>
-      <c r="T25" s="21">
+      <c r="T25" s="18">
         <v>12.097860320000004</v>
       </c>
-      <c r="U25" s="22">
+      <c r="U25" s="19">
         <v>20.131699999999999</v>
       </c>
     </row>
@@ -2324,16 +2360,16 @@
       <c r="Q26" s="12">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="20">
         <v>125</v>
       </c>
-      <c r="S26" s="23">
+      <c r="S26" s="20">
         <v>3.31711</v>
       </c>
-      <c r="T26" s="23">
+      <c r="T26" s="20">
         <v>3.8854914399999987</v>
       </c>
-      <c r="U26" s="24">
+      <c r="U26" s="21">
         <v>4.8229600000000001</v>
       </c>
     </row>
@@ -2390,16 +2426,16 @@
       <c r="Q27" s="12">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="R27" s="21">
+      <c r="R27" s="18">
         <v>125</v>
       </c>
-      <c r="S27" s="21">
+      <c r="S27" s="18">
         <v>15.666499999999999</v>
       </c>
-      <c r="T27" s="21">
+      <c r="T27" s="18">
         <v>26.932251999999998</v>
       </c>
-      <c r="U27" s="22">
+      <c r="U27" s="19">
         <v>178.05</v>
       </c>
     </row>
@@ -2456,16 +2492,16 @@
       <c r="Q28" s="12">
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="R28" s="23">
+      <c r="R28" s="20">
         <v>125</v>
       </c>
-      <c r="S28" s="23">
+      <c r="S28" s="20">
         <v>16.520099999999999</v>
       </c>
-      <c r="T28" s="23">
+      <c r="T28" s="20">
         <v>31.03646079999999</v>
       </c>
-      <c r="U28" s="24">
+      <c r="U28" s="21">
         <v>153.88399999999999</v>
       </c>
     </row>
@@ -2522,16 +2558,16 @@
       <c r="Q29" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="R29" s="21">
+      <c r="R29" s="18">
         <v>125</v>
       </c>
-      <c r="S29" s="21">
+      <c r="S29" s="18">
         <v>8.0663199999999993</v>
       </c>
-      <c r="T29" s="21">
+      <c r="T29" s="18">
         <v>11.175112719999994</v>
       </c>
-      <c r="U29" s="22">
+      <c r="U29" s="19">
         <v>16.129100000000001</v>
       </c>
     </row>
@@ -2588,16 +2624,16 @@
       <c r="Q30" s="12">
         <v>1.9E-2</v>
       </c>
-      <c r="R30" s="23">
+      <c r="R30" s="20">
         <v>125</v>
       </c>
-      <c r="S30" s="23">
+      <c r="S30" s="20">
         <v>41.654299999999999</v>
       </c>
-      <c r="T30" s="23">
+      <c r="T30" s="20">
         <v>74.429258400000023</v>
       </c>
-      <c r="U30" s="24">
+      <c r="U30" s="21">
         <v>655.53800000000001</v>
       </c>
     </row>
@@ -2654,16 +2690,16 @@
       <c r="Q31" s="12">
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="R31" s="21">
+      <c r="R31" s="18">
         <v>125</v>
       </c>
-      <c r="S31" s="21">
+      <c r="S31" s="18">
         <v>41.891300000000001</v>
       </c>
-      <c r="T31" s="21">
+      <c r="T31" s="18">
         <v>150.06952959999995</v>
       </c>
-      <c r="U31" s="22">
+      <c r="U31" s="19">
         <v>1681.32</v>
       </c>
     </row>
@@ -2720,16 +2756,16 @@
       <c r="Q32" s="12">
         <v>3.6000000000000004E-2</v>
       </c>
-      <c r="R32" s="23">
+      <c r="R32" s="20">
         <v>125</v>
       </c>
-      <c r="S32" s="23">
+      <c r="S32" s="20">
         <v>14.578000000000001</v>
       </c>
-      <c r="T32" s="23">
+      <c r="T32" s="20">
         <v>23.339043999999987</v>
       </c>
-      <c r="U32" s="24">
+      <c r="U32" s="21">
         <v>34.558500000000002</v>
       </c>
     </row>
@@ -2786,16 +2822,16 @@
       <c r="Q33" s="12">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="R33" s="21">
+      <c r="R33" s="18">
         <v>125</v>
       </c>
-      <c r="S33" s="21">
+      <c r="S33" s="18">
         <v>134.601</v>
       </c>
-      <c r="T33" s="21">
+      <c r="T33" s="18">
         <v>910.43100799999979</v>
       </c>
-      <c r="U33" s="22">
+      <c r="U33" s="19">
         <v>16995.3</v>
       </c>
     </row>
@@ -2852,16 +2888,16 @@
       <c r="Q34" s="12">
         <v>0.04</v>
       </c>
-      <c r="R34" s="23">
+      <c r="R34" s="20">
         <v>375</v>
       </c>
-      <c r="S34" s="23">
+      <c r="S34" s="20">
         <v>6.8121800000000006</v>
       </c>
-      <c r="T34" s="23">
+      <c r="T34" s="20">
         <v>11.76670208</v>
       </c>
-      <c r="U34" s="24">
+      <c r="U34" s="21">
         <v>28.186699999999998</v>
       </c>
     </row>
@@ -2918,16 +2954,16 @@
       <c r="Q35" s="12">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="R35" s="21">
+      <c r="R35" s="18">
         <v>375</v>
       </c>
-      <c r="S35" s="21">
+      <c r="S35" s="18">
         <v>0.71468699999999996</v>
       </c>
-      <c r="T35" s="21">
+      <c r="T35" s="18">
         <v>4.4493516399999979</v>
       </c>
-      <c r="U35" s="22">
+      <c r="U35" s="19">
         <v>8.2983399999999996</v>
       </c>
     </row>
@@ -2984,16 +3020,16 @@
       <c r="Q36" s="12">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="R36" s="23">
+      <c r="R36" s="20">
         <v>375</v>
       </c>
-      <c r="S36" s="23">
+      <c r="S36" s="20">
         <v>18.935400000000001</v>
       </c>
-      <c r="T36" s="23">
+      <c r="T36" s="20">
         <v>84.606281333333314</v>
       </c>
-      <c r="U36" s="24">
+      <c r="U36" s="21">
         <v>545.59400000000005</v>
       </c>
     </row>
@@ -3050,16 +3086,16 @@
       <c r="Q37" s="12">
         <v>6.8999999999999992E-2</v>
       </c>
-      <c r="R37" s="21">
+      <c r="R37" s="18">
         <v>375</v>
       </c>
-      <c r="S37" s="21">
+      <c r="S37" s="18">
         <v>13.670699999999998</v>
       </c>
-      <c r="T37" s="21">
+      <c r="T37" s="18">
         <v>44.644739199999975</v>
       </c>
-      <c r="U37" s="22">
+      <c r="U37" s="19">
         <v>234.41899999999998</v>
       </c>
     </row>
@@ -3116,16 +3152,16 @@
       <c r="Q38" s="12">
         <v>2.0190000000000001</v>
       </c>
-      <c r="R38" s="23">
+      <c r="R38" s="20">
         <v>375</v>
       </c>
-      <c r="S38" s="23">
+      <c r="S38" s="20">
         <v>3.2667600000000001</v>
       </c>
-      <c r="T38" s="23">
+      <c r="T38" s="20">
         <v>8.6770603999999967</v>
       </c>
-      <c r="U38" s="24">
+      <c r="U38" s="21">
         <v>17.1465</v>
       </c>
     </row>
@@ -3182,16 +3218,16 @@
       <c r="Q39" s="12">
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="R39" s="21">
+      <c r="R39" s="18">
         <v>375</v>
       </c>
-      <c r="S39" s="21">
+      <c r="S39" s="18">
         <v>43.182499999999997</v>
       </c>
-      <c r="T39" s="21">
+      <c r="T39" s="18">
         <v>824.36544053333319</v>
       </c>
-      <c r="U39" s="22">
+      <c r="U39" s="19">
         <v>19479.399999999998</v>
       </c>
     </row>
@@ -3248,16 +3284,16 @@
       <c r="Q40" s="12">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="R40" s="23">
+      <c r="R40" s="20">
         <v>375</v>
       </c>
-      <c r="S40" s="23">
+      <c r="S40" s="20">
         <v>44.307299999999998</v>
       </c>
-      <c r="T40" s="23">
+      <c r="T40" s="20">
         <v>309.84588480000002</v>
       </c>
-      <c r="U40" s="24">
+      <c r="U40" s="21">
         <v>7116.4500000000007</v>
       </c>
     </row>
@@ -3314,16 +3350,16 @@
       <c r="Q41" s="12">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="R41" s="21">
+      <c r="R41" s="18">
         <v>375</v>
       </c>
-      <c r="S41" s="21">
+      <c r="S41" s="18">
         <v>3.9438700000000004</v>
       </c>
-      <c r="T41" s="21">
+      <c r="T41" s="18">
         <v>22.14598311999999</v>
       </c>
-      <c r="U41" s="22">
+      <c r="U41" s="19">
         <v>35.573300000000003</v>
       </c>
     </row>
@@ -3380,21 +3416,21 @@
       <c r="Q42" s="15">
         <v>0.16699999999999998</v>
       </c>
-      <c r="R42" s="23">
+      <c r="R42" s="20">
         <v>374</v>
       </c>
-      <c r="S42" s="23">
+      <c r="S42" s="20">
         <v>186.89700000000002</v>
       </c>
-      <c r="T42" s="23">
+      <c r="T42" s="20">
         <v>14962.915789333329</v>
       </c>
-      <c r="U42" s="24">
+      <c r="U42" s="21">
         <v>600003</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -3406,7 +3442,7 @@
       <c r="E43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="27" t="s">
+      <c r="F43" s="22" t="s">
         <v>20</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -3418,7 +3454,7 @@
       <c r="I43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J43" s="22" t="s">
         <v>20</v>
       </c>
       <c r="K43" s="2" t="s">
@@ -3430,7 +3466,7 @@
       <c r="M43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N43" s="27" t="s">
+      <c r="N43" s="22" t="s">
         <v>20</v>
       </c>
       <c r="O43" s="2" t="s">
@@ -4428,6 +4464,691 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6F7C63-A5F8-43F7-A33B-A8CD8F566FAF}">
+  <dimension ref="B1:V33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B4" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B5" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0</v>
+      </c>
+      <c r="D5" s="28">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="28">
+        <v>1.880799999999996E-2</v>
+      </c>
+      <c r="F5" s="28">
+        <v>0.23900000000000002</v>
+      </c>
+      <c r="G5" s="28">
+        <v>57.692300000000003</v>
+      </c>
+      <c r="H5" s="28">
+        <v>834.59762999999987</v>
+      </c>
+      <c r="I5" s="28">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B6" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="28">
+        <v>32</v>
+      </c>
+      <c r="D6" s="28">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="28">
+        <v>1.4661333333333318E-2</v>
+      </c>
+      <c r="F6" s="28">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G6" s="28">
+        <v>50</v>
+      </c>
+      <c r="H6" s="28">
+        <v>617.98596466666663</v>
+      </c>
+      <c r="I6" s="28">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="28">
+        <v>55</v>
+      </c>
+      <c r="D7" s="28">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E7" s="28">
+        <v>1.4770666666666614E-2</v>
+      </c>
+      <c r="F7" s="28">
+        <v>6.8999999999999992E-2</v>
+      </c>
+      <c r="G7" s="28">
+        <v>0</v>
+      </c>
+      <c r="H7" s="28">
+        <v>372.70585866666664</v>
+      </c>
+      <c r="I7" s="28">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="28">
+        <v>175</v>
+      </c>
+      <c r="D8" s="28">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E8" s="28">
+        <v>1.7783999999999977E-2</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0.04</v>
+      </c>
+      <c r="G8" s="28">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <v>185.65302240000003</v>
+      </c>
+      <c r="I8" s="28">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="28">
+        <v>375</v>
+      </c>
+      <c r="D9" s="28">
+        <v>6.8121800000000006</v>
+      </c>
+      <c r="E9" s="28">
+        <v>11.76670208</v>
+      </c>
+      <c r="F9" s="28">
+        <v>28.186699999999998</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B13" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E13" s="28">
+        <v>2.1719999999999962E-2</v>
+      </c>
+      <c r="F13" s="28">
+        <v>0.121</v>
+      </c>
+      <c r="G13" s="28">
+        <v>68.421099999999996</v>
+      </c>
+      <c r="H13" s="28">
+        <v>1183.1473999999996</v>
+      </c>
+      <c r="I13" s="28">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="28">
+        <v>8</v>
+      </c>
+      <c r="D14" s="28">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E14" s="28">
+        <v>1.8487999999999956E-2</v>
+      </c>
+      <c r="F14" s="28">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G14" s="28">
+        <v>61.538499999999999</v>
+      </c>
+      <c r="H14" s="28">
+        <v>829.69579213973782</v>
+      </c>
+      <c r="I14" s="28">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B15" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="28">
+        <v>14</v>
+      </c>
+      <c r="D15" s="28">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E15" s="28">
+        <v>2.1645333333333298E-2</v>
+      </c>
+      <c r="F15" s="28">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0</v>
+      </c>
+      <c r="H15" s="28">
+        <v>481.46310611353709</v>
+      </c>
+      <c r="I15" s="28">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B16" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="28">
+        <v>90</v>
+      </c>
+      <c r="D16" s="28">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="E16" s="28">
+        <v>2.0319999999999963E-2</v>
+      </c>
+      <c r="F16" s="28">
+        <v>6.8999999999999992E-2</v>
+      </c>
+      <c r="G16" s="28">
+        <v>0</v>
+      </c>
+      <c r="H16" s="28">
+        <v>238.95319558951962</v>
+      </c>
+      <c r="I16" s="28">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="28">
+        <v>375</v>
+      </c>
+      <c r="D17" s="28">
+        <v>13.670699999999998</v>
+      </c>
+      <c r="E17" s="28">
+        <v>44.644739199999975</v>
+      </c>
+      <c r="F17" s="28">
+        <v>234.41899999999998</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="28">
+        <v>0</v>
+      </c>
+      <c r="D21" s="28">
+        <v>1.5000000000000001E-2</v>
+      </c>
+      <c r="E21" s="28">
+        <v>2.5994666666666638E-2</v>
+      </c>
+      <c r="F21" s="28">
+        <v>6.9999999999999993E-2</v>
+      </c>
+      <c r="G21" s="28">
+        <v>36.206899999999997</v>
+      </c>
+      <c r="H21" s="28">
+        <v>1243.0659126245851</v>
+      </c>
+      <c r="I21" s="28">
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="28">
+        <v>1</v>
+      </c>
+      <c r="D22" s="28">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E22" s="28">
+        <v>3.0487999999999977E-2</v>
+      </c>
+      <c r="F22" s="28">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="G22" s="28">
+        <v>77.777799999999999</v>
+      </c>
+      <c r="H22" s="28">
+        <v>852.59662591362132</v>
+      </c>
+      <c r="I22" s="28">
+        <v>5800</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="28">
+        <v>1</v>
+      </c>
+      <c r="D23" s="28">
+        <v>1.5000000000000001E-2</v>
+      </c>
+      <c r="E23" s="28">
+        <v>2.8530666666666642E-2</v>
+      </c>
+      <c r="F23" s="28">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G23" s="28">
+        <v>51.7241</v>
+      </c>
+      <c r="H23" s="28">
+        <v>468.86023853820586</v>
+      </c>
+      <c r="I23" s="28">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="28">
+        <v>25</v>
+      </c>
+      <c r="D24" s="28">
+        <v>1.5000000000000001E-2</v>
+      </c>
+      <c r="E24" s="28">
+        <v>3.2714666666666663E-2</v>
+      </c>
+      <c r="F24" s="28">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="G24" s="28">
+        <v>0</v>
+      </c>
+      <c r="H24" s="28">
+        <v>230.7150429235879</v>
+      </c>
+      <c r="I24" s="28">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="28">
+        <v>375</v>
+      </c>
+      <c r="D25" s="28">
+        <v>44.307299999999998</v>
+      </c>
+      <c r="E25" s="28">
+        <v>309.84588480000002</v>
+      </c>
+      <c r="F25" s="28">
+        <v>7116.4500000000007</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="28">
+        <v>1</v>
+      </c>
+      <c r="D29" s="28">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="E29" s="28">
+        <v>1.7858666666666637E-2</v>
+      </c>
+      <c r="F29" s="28">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G29" s="28">
+        <v>73.333299999999994</v>
+      </c>
+      <c r="H29" s="28">
+        <v>1602.4430811320753</v>
+      </c>
+      <c r="I29" s="28">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="28">
+        <v>106</v>
+      </c>
+      <c r="D30" s="28">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E30" s="28">
+        <v>1.4103999999999971E-2</v>
+      </c>
+      <c r="F30" s="28">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="G30" s="28">
+        <v>213.333</v>
+      </c>
+      <c r="H30" s="28">
+        <v>1189.1951132075471</v>
+      </c>
+      <c r="I30" s="28">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="28">
+        <v>138</v>
+      </c>
+      <c r="D31" s="28">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="E31" s="28">
+        <v>1.703199999999995E-2</v>
+      </c>
+      <c r="F31" s="28">
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="G31" s="28">
+        <v>100</v>
+      </c>
+      <c r="H31" s="28">
+        <v>689.02069811320757</v>
+      </c>
+      <c r="I31" s="28">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="28">
+        <v>270</v>
+      </c>
+      <c r="D32" s="28">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="E32" s="28">
+        <v>1.9474666666666623E-2</v>
+      </c>
+      <c r="F32" s="28">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G32" s="28">
+        <v>0</v>
+      </c>
+      <c r="H32" s="28">
+        <v>281.9279811320755</v>
+      </c>
+      <c r="I32" s="28">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="28">
+        <v>375</v>
+      </c>
+      <c r="D33" s="28">
+        <v>3.9438700000000004</v>
+      </c>
+      <c r="E33" s="28">
+        <v>22.14598311999999</v>
+      </c>
+      <c r="F33" s="28">
+        <v>35.573300000000003</v>
+      </c>
+      <c r="G33" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A3:Q61"/>
   <sheetViews>
@@ -4707,30 +5428,30 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="16" t="s">
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="16" t="s">
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="16" t="s">
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="18"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="25"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">

</xml_diff>